<commit_message>
Added more quests, items, update guide quests and lots of other changes.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Monsters/weekly-monsters-delusional-memories.xlsx
+++ b/resources/data-imports/Monsters/weekly-monsters-delusional-memories.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="84">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -199,6 +199,9 @@
     <t xml:space="preserve">13498483-26996966</t>
   </si>
   <si>
+    <t xml:space="preserve">Candle of Absolution</t>
+  </si>
+  <si>
     <t xml:space="preserve">Judge of Shattered Faith</t>
   </si>
   <si>
@@ -223,6 +226,9 @@
     <t xml:space="preserve">29876997-59753994</t>
   </si>
   <si>
+    <t xml:space="preserve">Metalic Idol of God</t>
+  </si>
+  <si>
     <t xml:space="preserve">Judge of the Forsaken Flame</t>
   </si>
   <si>
@@ -245,6 +251,9 @@
   </si>
   <si>
     <t xml:space="preserve">66128537-132257075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Histories of Heretical Alchemy</t>
   </si>
   <si>
     <t xml:space="preserve">Judge of Delirious Peace</t>
@@ -354,7 +363,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -369,6 +378,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -565,8 +578,8 @@
   </sheetPr>
   <dimension ref="A1:AX16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AQ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AQ2" activeCellId="0" sqref="AQ2:AS16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AK1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AN10" activeCellId="0" sqref="AN10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -577,7 +590,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="18.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.71"/>
@@ -601,7 +614,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="31.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="24.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="42" style="1" width="16.71"/>
@@ -1278,8 +1291,11 @@
       <c r="AL5" s="1" t="n">
         <v>0.165359097343183</v>
       </c>
+      <c r="AM5" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="AN5" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO5" s="1" t="s">
         <v>52</v>
@@ -1305,7 +1321,7 @@
         <v>529</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>3657157862.02662</v>
@@ -1371,10 +1387,10 @@
         <v>0</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AA6" s="3" t="n">
         <v>3657157862.02662</v>
@@ -1436,7 +1452,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>4044169278.45986</v>
@@ -1502,10 +1518,10 @@
         <v>0</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AA7" s="3" t="n">
         <v>4044169278.45986</v>
@@ -1567,7 +1583,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>4472135404.01432</v>
@@ -1633,10 +1649,10 @@
         <v>0</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AA8" s="3" t="n">
         <v>4472135404.01432</v>
@@ -1698,7 +1714,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>4945390188.87332</v>
@@ -1764,10 +1780,10 @@
         <v>0</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AA9" s="3" t="n">
         <v>4945390188.87332</v>
@@ -1805,8 +1821,11 @@
       <c r="AL9" s="1" t="n">
         <v>0.247269509443666</v>
       </c>
+      <c r="AM9" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="AN9" s="1" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="AO9" s="1" t="s">
         <v>52</v>
@@ -1829,7 +1848,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>5468726214.83047</v>
@@ -1895,10 +1914,10 @@
         <v>0</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AA10" s="3" t="n">
         <v>5468726214.83047</v>
@@ -1960,7 +1979,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>6047443229.06247</v>
@@ -2026,10 +2045,10 @@
         <v>0</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="AA11" s="3" t="n">
         <v>6047443229.06247</v>
@@ -2091,7 +2110,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>6687401813.89155</v>
@@ -2157,10 +2176,10 @@
         <v>0</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AA12" s="3" t="n">
         <v>6687401813.89155</v>
@@ -2222,7 +2241,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>7395082736.04299</v>
@@ -2288,10 +2307,10 @@
         <v>0</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA13" s="3" t="n">
         <v>7395082736.04299</v>
@@ -2329,8 +2348,11 @@
       <c r="AL13" s="1" t="n">
         <v>0.36975413680215</v>
       </c>
+      <c r="AM13" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="AN13" s="1" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AO13" s="1" t="s">
         <v>52</v>
@@ -2353,7 +2375,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>8177652576.41927</v>
@@ -2419,10 +2441,10 @@
         <v>0</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AA14" s="3" t="n">
         <v>8177652576.41927</v>
@@ -2484,7 +2506,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>9043036305.01369</v>
@@ -2550,10 +2572,10 @@
         <v>0</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="AA15" s="3" t="n">
         <v>9043036305.01369</v>
@@ -2615,7 +2637,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>9999997535.91915</v>
@@ -2681,10 +2703,10 @@
         <v>0</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="AA16" s="3" t="n">
         <v>9999997535.91915</v>

</xml_diff>